<commit_message>
First set of changes to match EGD report. No code, only text for now.
</commit_message>
<xml_diff>
--- a/indicators/NO_URGR_010-031/metadata.xlsx
+++ b/indicators/NO_URGR_010-031/metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.grainger\Documents\Projects_in_development\ecRxiv\indicators\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\61546-01_fu_intern_sylvie_clappe\ecRixv_urbangreen\ecRxiv_urbangreen\indicators\NO_URGR_010-031\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433C71A1-6EC0-4AA9-AEBA-19C7C8982435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A9E935-DF16-4D5D-AF2C-54557A3966C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="156" windowWidth="23040" windowHeight="12204" activeTab="1" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5774BAF6-AFFD-43CB-8AE5-DFBA2C21B702}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="209">
   <si>
     <t>indicatorID</t>
   </si>
@@ -694,6 +694,21 @@
   </si>
   <si>
     <t>A2 - Chemical State characteristics</t>
+  </si>
+  <si>
+    <t>URGR_013_to_031</t>
+  </si>
+  <si>
+    <t>Urban Green</t>
+  </si>
+  <si>
+    <t>First draft version, work in progress</t>
+  </si>
+  <si>
+    <t>Clappe, S., Czúcz, B.</t>
+  </si>
+  <si>
+    <t>National scale - Aggregated at Regional level</t>
   </si>
 </sst>
 </file>
@@ -1153,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78FF33B-C37D-487F-A5F6-37AB2202A4CF}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,6 +1198,9 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>199</v>
       </c>
@@ -1194,7 +1212,9 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>205</v>
+      </c>
       <c r="C3" s="2" t="s">
         <v>201</v>
       </c>
@@ -1206,7 +1226,9 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
@@ -1216,7 +1238,9 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
@@ -1226,7 +1250,9 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
@@ -1235,7 +1261,9 @@
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>170</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1247,7 +1275,9 @@
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>139</v>
       </c>
@@ -1259,7 +1289,9 @@
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1272,7 +1304,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="2">
-        <v>1901</v>
+        <v>2024</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>25</v>
@@ -1283,7 +1315,9 @@
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>2025</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>19</v>
       </c>
@@ -1319,7 +1353,9 @@
       <c r="A14" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>206</v>
+      </c>
       <c r="C14" s="2" t="s">
         <v>169</v>
       </c>
@@ -1330,7 +1366,7 @@
         <v>186</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>183</v>
@@ -1357,7 +1393,9 @@
       <c r="A17" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>193</v>
+      </c>
       <c r="C17" s="2" t="s">
         <v>191</v>
       </c>
@@ -1369,7 +1407,9 @@
       <c r="A18" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>208</v>
+      </c>
       <c r="C18" s="2" t="s">
         <v>198</v>
       </c>
@@ -1434,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38FBD06A-F7D1-4345-BCDF-E89F4B8A4AD5}">
   <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>